<commit_message>
Se añadio Casosde Prueba a  la funcionalidad Agregar Proveedor
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M5.xlsx
+++ b/2-Desarrollo/SCIP/pruebas-calidad/SCIP-DCS-M5.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b6b49da01230f2/Documentos/proyecto wong/Softgenix-Peru/2-Desarrollo/SCIP/pruebas-calidad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_8BF91C39AE0E0FE7D0D966DCD60DF29A91746BA8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C8E03D5-4F1C-42D5-BFFD-9BACFE0C2BFF}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_8BF91C39AE0E0FE7D0D966DCD60DF29A91746BA8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89133408-79B2-423C-A681-1D6097093522}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="17925" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Clases de equivalenciaAgrega" sheetId="1" r:id="rId1"/>
-    <sheet name="2.0CP Buscar Producto" sheetId="2" r:id="rId2"/>
+    <sheet name="CP Agregar Proveedor" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>CLASES VÁLIDAS</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Código</t>
   </si>
   <si>
-    <t>AGREGAR USUARIO</t>
-  </si>
-  <si>
     <t>CONDICIONES DE ENTRADA</t>
   </si>
   <si>
@@ -61,21 +58,6 @@
     <t>Clases de equivalencia</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t>Tipo de Perfil</t>
-  </si>
-  <si>
-    <t>Foto</t>
-  </si>
-  <si>
     <t>Resultado esperado</t>
   </si>
   <si>
@@ -94,30 +76,6 @@
     <t>CP04</t>
   </si>
   <si>
-    <t>CP05</t>
-  </si>
-  <si>
-    <t>CP06</t>
-  </si>
-  <si>
-    <t>CP07</t>
-  </si>
-  <si>
-    <t>CP08</t>
-  </si>
-  <si>
-    <t>CP09</t>
-  </si>
-  <si>
-    <t>CP10</t>
-  </si>
-  <si>
-    <t>CP11</t>
-  </si>
-  <si>
-    <t>CP12</t>
-  </si>
-  <si>
     <t>Codigo</t>
   </si>
   <si>
@@ -176,13 +134,49 @@
   </si>
   <si>
     <t>CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>AGREGAR PROVEEDOR</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>Agregado exitoso</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;03&gt;,CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>GRUPO HILOS</t>
+  </si>
+  <si>
+    <t>Proveedor creado satisfactoriamente</t>
+  </si>
+  <si>
+    <t>Cueros Miguel</t>
+  </si>
+  <si>
+    <t>agregado erroneo</t>
+  </si>
+  <si>
+    <t>CENV&lt;01&gt;,CEV&lt;02&gt;,CEV&lt;03&gt;,CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>codigo no valido</t>
+  </si>
+  <si>
+    <t>CEV&lt;01&gt;,CENV&lt;02&gt;,CEV&lt;03&gt;,CEV&lt;04&gt;</t>
+  </si>
+  <si>
+    <t>Agregar codigo valido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -193,47 +187,43 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -259,8 +249,14 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,32 +287,8 @@
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4A7D6"/>
-        <bgColor rgb="FFB4A7D6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8AF"/>
-        <bgColor rgb="FFE6B8AF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF9CB9C"/>
-        <bgColor rgb="FFF9CB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9FC5E8"/>
-        <bgColor rgb="FF9FC5E8"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -365,32 +337,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -408,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -420,137 +366,92 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P985"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -848,63 +749,63 @@
     <row r="2" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="40" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="40" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="33"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>35</v>
+      <c r="B6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -916,21 +817,21 @@
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="48"/>
-      <c r="C7" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="46" t="s">
-        <v>40</v>
+      <c r="B7" s="16"/>
+      <c r="C7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -938,19 +839,19 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="32"/>
+      <c r="O7" s="21"/>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>42</v>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -958,27 +859,27 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="20"/>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>42</v>
+      <c r="B9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -986,25 +887,25 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="32"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
-      <c r="C10" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>42</v>
+      <c r="B10" s="16"/>
+      <c r="C10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1012,19 +913,19 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="33"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>42</v>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1032,7 +933,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="32"/>
+      <c r="O11" s="21"/>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1042,7 +943,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="33"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2101,12 +2002,6 @@
     <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -2116,6 +2011,12 @@
     <mergeCell ref="O9:O10"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2125,262 +2026,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L991"/>
+  <dimension ref="A1:L977"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" customWidth="1"/>
     <col min="10" max="28" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D2" s="37" t="s">
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="35"/>
+      <c r="C4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
     </row>
-    <row r="3" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="C5" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="25">
+        <v>123456789</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="C6" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="25">
+        <v>124566</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="31"/>
+      <c r="I6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="C7" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="36">
+        <v>-12345</v>
+      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="36"/>
+      <c r="I7" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="35"/>
+      <c r="C8" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
     </row>
-    <row r="4" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-    </row>
-    <row r="5" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-    </row>
-    <row r="14" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:12" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="29"/>
-    </row>
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3343,25 +3171,25 @@
     <row r="975" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="976" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="977" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="978" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="979" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="980" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="981" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="982" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="983" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="984" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="17">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J6:L6"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>